<commit_message>
parameter selection for svr
</commit_message>
<xml_diff>
--- a/linear_regression/stats_lr_results.xlsx
+++ b/linear_regression/stats_lr_results.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\regression_models\linear_regression\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>consumption</t>
   </si>
@@ -68,23 +72,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -99,26 +104,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -406,20 +428,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,207 +465,207 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.7188110993627581</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>0.71881109936275811</v>
+      </c>
+      <c r="C2">
         <v>0.7088256980617198</v>
       </c>
-      <c r="D2" t="n">
-        <v>59.23076083052669</v>
-      </c>
-      <c r="E2" t="n">
-        <v>53.89909400418436</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.4514849005630948</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="D2">
+        <v>59.230760830526691</v>
+      </c>
+      <c r="E2">
+        <v>53.899094004184363</v>
+      </c>
+      <c r="F2">
+        <v>0.45148490056309482</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>0.7417305322273644</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.7325590312411203</v>
-      </c>
-      <c r="D3" t="n">
-        <v>74.88080127853422</v>
-      </c>
-      <c r="E3" t="n">
-        <v>17.8363572853791</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.2652496338654488</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3">
+        <v>0.73255903124112032</v>
+      </c>
+      <c r="D3">
+        <v>74.880801278534221</v>
+      </c>
+      <c r="E3">
+        <v>17.836357285379101</v>
+      </c>
+      <c r="F3">
+        <v>0.26524963386544881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>0.1371777824980458</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0.1065377889788004</v>
       </c>
-      <c r="D4" t="n">
-        <v>192.8944412055166</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
+        <v>192.89444120551661</v>
+      </c>
+      <c r="E4">
         <v>5.416934245611758</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>-1.659851547935193</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.69426304934243</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.6834059133105561</v>
-      </c>
-      <c r="D5" t="n">
-        <v>59.60805097859762</v>
-      </c>
-      <c r="E5" t="n">
-        <v>16.86524781805026</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.3724013245957969</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="B5">
+        <v>0.69426304934242999</v>
+      </c>
+      <c r="C5">
+        <v>0.68340591331055611</v>
+      </c>
+      <c r="D5">
+        <v>59.608050978597618</v>
+      </c>
+      <c r="E5">
+        <v>16.865247818050261</v>
+      </c>
+      <c r="F5">
+        <v>0.37240132459579689</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="n">
-        <v>0.6884342872885985</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.6773701639678811</v>
-      </c>
-      <c r="D6" t="n">
-        <v>78.37621302313514</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="B6">
+        <v>0.68843428728859846</v>
+      </c>
+      <c r="C6">
+        <v>0.67737016396788108</v>
+      </c>
+      <c r="D6">
+        <v>78.376213023135136</v>
+      </c>
+      <c r="E6">
         <v>11.61035108857997</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.3381955166993686</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6">
+        <v>0.33819551669936859</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.7303306295231853</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.7207543024465939</v>
-      </c>
-      <c r="D7" t="n">
-        <v>58.15569715663266</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="B7">
+        <v>0.73033062952318528</v>
+      </c>
+      <c r="C7">
+        <v>0.72075430244659389</v>
+      </c>
+      <c r="D7">
+        <v>58.155697156632662</v>
+      </c>
+      <c r="E7">
         <v>16.55153603229817</v>
       </c>
-      <c r="F7" t="n">
-        <v>0.4142783177429666</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7">
+        <v>0.41427831774296658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>0.7714019768679603</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.7632841493419646</v>
-      </c>
-      <c r="D8" t="n">
-        <v>52.89009372467925</v>
-      </c>
-      <c r="E8" t="n">
+      <c r="C8">
+        <v>0.76328414934196465</v>
+      </c>
+      <c r="D8">
+        <v>52.890093724679247</v>
+      </c>
+      <c r="E8">
         <v>41.15422562154388</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>0.4116982166704195</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="n">
-        <v>0.5928755272960602</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="B9">
+        <v>0.59287552729606019</v>
+      </c>
+      <c r="C9">
         <v>0.5784179821006078</v>
       </c>
-      <c r="D9" t="n">
-        <v>193.2247030669037</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="D9">
+        <v>193.22470306690369</v>
+      </c>
+      <c r="E9">
         <v>21.56715490246312</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>0.6375045404042724</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.6340678927244987</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.6210731445968176</v>
-      </c>
-      <c r="D10" t="n">
-        <v>73.86946935057439</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="B10">
+        <v>0.63406789272449871</v>
+      </c>
+      <c r="C10">
+        <v>0.62107314459681762</v>
+      </c>
+      <c r="D10">
+        <v>73.869469350574391</v>
+      </c>
+      <c r="E10">
         <v>12.77831915707211</v>
       </c>
-      <c r="F10" t="n">
-        <v>0.2231724076327841</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10">
+        <v>0.22317240763278409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.8265135632720939</v>
-      </c>
-      <c r="C11" t="n">
+      <c r="B11">
+        <v>0.82651356327209391</v>
+      </c>
+      <c r="C11">
         <v>0.8203528233314723</v>
       </c>
-      <c r="D11" t="n">
-        <v>41.65912382935412</v>
-      </c>
-      <c r="E11" t="n">
-        <v>139.2212374725023</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.4235366338115352</v>
+      <c r="D11">
+        <v>41.659123829354122</v>
+      </c>
+      <c r="E11">
+        <v>139.22123747250231</v>
+      </c>
+      <c r="F11">
+        <v>0.42353663381153522</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>